<commit_message>
added knowledge about pytest and node
</commit_message>
<xml_diff>
--- a/selenium/example.xlsx
+++ b/selenium/example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="187">
   <si>
     <t>PREMIUMTECH_PL</t>
   </si>
@@ -569,6 +569,39 @@
   </si>
   <si>
     <t>87 (coil whine) &lt;xeon&gt;</t>
+  </si>
+  <si>
+    <t>84 (ok) &lt;xeon&gt;</t>
+  </si>
+  <si>
+    <t>kuplatopa</t>
+  </si>
+  <si>
+    <t>7,3k</t>
+  </si>
+  <si>
+    <t>jest/5k</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>9,5k</t>
+  </si>
+  <si>
+    <t>84 (troche glosna) &lt;xeon&gt;</t>
+  </si>
+  <si>
+    <t>6k</t>
+  </si>
+  <si>
+    <t>88 (b.ok)</t>
+  </si>
+  <si>
+    <t>78 (żle, coil)</t>
+  </si>
+  <si>
+    <t>84 (przy malym obc.)</t>
   </si>
 </sst>
 </file>
@@ -773,10 +806,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1092,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2738,7 +2771,7 @@
   <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C27" sqref="C11:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2770,7 +2803,7 @@
       <c r="D3">
         <v>2015</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>166</v>
       </c>
       <c r="F3" t="s">
@@ -2782,7 +2815,7 @@
       <c r="H3" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2802,14 +2835,14 @@
       <c r="H4" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="23" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C5" s="22"/>
       <c r="H5" s="23"/>
-      <c r="I5" s="22"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -2821,7 +2854,7 @@
       <c r="D6">
         <v>2015</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>170</v>
       </c>
       <c r="G6">
@@ -2830,7 +2863,7 @@
       <c r="H6" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2847,10 +2880,10 @@
       <c r="G7">
         <v>2500</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="23" t="s">
         <v>171</v>
       </c>
       <c r="J7" t="s">
@@ -2860,12 +2893,12 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" s="22"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="22"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C9" s="22"/>
       <c r="H9" s="23"/>
-      <c r="I9" s="22"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -2877,11 +2910,21 @@
       <c r="D10">
         <v>2015</v>
       </c>
+      <c r="E10" t="s">
+        <v>176</v>
+      </c>
       <c r="G10">
         <v>2800</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="22"/>
+      <c r="H10" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C11" s="22">
@@ -2890,16 +2933,23 @@
       <c r="D11">
         <v>2017</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="G11">
         <v>2800</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="22"/>
+      <c r="H11" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C12" s="22"/>
       <c r="H12" s="23"/>
-      <c r="I12" s="22"/>
+      <c r="I12" s="23"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C13" s="22">
@@ -2908,11 +2958,18 @@
       <c r="D13">
         <v>2015</v>
       </c>
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
       <c r="G13">
         <v>1800</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="22"/>
+      <c r="H13" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C14" s="22">
@@ -2921,57 +2978,93 @@
       <c r="D14">
         <v>2017</v>
       </c>
+      <c r="E14" t="s">
+        <v>182</v>
+      </c>
       <c r="G14">
         <v>1800</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="22"/>
+      <c r="H14" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C15" s="22"/>
       <c r="H15" s="23"/>
-      <c r="I15" s="22"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C16" s="22">
-        <v>3500</v>
+        <v>3510</v>
       </c>
       <c r="D16">
-        <v>2015</v>
+        <v>2016</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="G16">
         <v>2200</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="22"/>
+      <c r="H16" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="22">
-        <v>3510</v>
+        <v>3520</v>
       </c>
       <c r="D17">
         <v>2017</v>
       </c>
+      <c r="E17" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G17">
         <v>2200</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="22"/>
+      <c r="H17" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" s="22"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="22"/>
+      <c r="C18" s="22">
+        <v>3530</v>
+      </c>
+      <c r="D18">
+        <v>2018</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18">
+        <v>2300</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="22"/>
       <c r="H19" s="23"/>
-      <c r="I19" s="22"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" s="22"/>
       <c r="H20" s="23"/>
-      <c r="I20" s="22"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" s="22"/>

</xml_diff>